<commit_message>
new fields visible: URL, amount paid, and entity filtering
</commit_message>
<xml_diff>
--- a/phase-two-taxes-8-17.xlsx
+++ b/phase-two-taxes-8-17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwoody/workspace/ongoing-projects/taxes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69A9172-6720-954A-8336-1C3B1462535F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD9784A-A6A8-F74B-BA56-64B50CA7BA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3560" yWindow="-21100" windowWidth="34200" windowHeight="18460" xr2:uid="{1AC72A25-3CAC-4547-8CAF-80A286E701F6}"/>
   </bookViews>
@@ -3194,8 +3194,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="188" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="83" workbookViewId="0">
+      <selection activeCell="H146" sqref="H146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3210,7 +3210,7 @@
     <col min="15" max="15" width="17.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>42</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>56</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>66</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>74</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>77</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>80</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>83</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>84</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>85</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>97</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>99</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>100</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>104</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>107</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>110</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>113</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>117</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>121</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>125</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>128</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>131</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>132</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>136</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>138</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>142</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>145</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>146</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>149</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>154</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>157</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>160</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>163</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>166</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>169</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>171</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>172</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>176</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>181</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>182</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>188</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>190</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>191</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>196</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>198</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>199</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>203</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>206</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>209</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>212</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>213</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>216</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>220</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>221</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>225</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>229</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>231</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>235</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>237</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>239</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>241</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>242</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>246</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>250</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>260</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>261</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>265</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>268</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>281</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>293</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="204" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="204" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>305</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>313</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>335</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>341</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>344</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>348</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>349</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>353</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>357</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>360</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>363</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>365</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>368</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>371</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>375</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" ht="104" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>380</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>383</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>389</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>392</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="306" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" ht="306" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>393</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>396</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>400</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="69" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" ht="69" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>403</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>406</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>410</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>414</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>420</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>424</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>427</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>431</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>434</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>437</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>440</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>441</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>444</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>447</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>449</v>
       </c>
@@ -8023,7 +8023,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>285</v>
       </c>
@@ -8556,7 +8556,7 @@
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:K3 G5:K5 G7:K22 G26:K28 G30:K32 G34:J34 G35:K35 J36:K47 G36:H52 J48:J52 K49 G53:K55 G56:I56 K56 G57:K62 J63:K63 G63:H66 K64 J65:K66 G67:K70 G71:H71 J71:K71 G72:K1048576">
+  <conditionalFormatting sqref="G72:K1048576 G1:K3 G5:K5 G7:K22 G26:K28 G30:K32 G34:J34 G35:K35 J36:K47 G36:H52 J48:J52 K49 G53:K55 G56:I56 K56 G57:K62 J63:K63 G63:H66 K64 J65:K66 G67:K70 G71:H71 J71:K71">
     <cfRule type="containsBlanks" dxfId="13" priority="26">
       <formula>LEN(TRIM(G1))=0</formula>
     </cfRule>
@@ -8610,8 +8610,6 @@
     <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(O125))=0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O125">
     <cfRule type="containsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(O125))=0</formula>
     </cfRule>

</xml_diff>